<commit_message>
fixes ver no reelec
</commit_message>
<xml_diff>
--- a/data/fechasEleccionesMexicoDesde1994.xlsx
+++ b/data/fechasEleccionesMexicoDesde1994.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3719" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3720" uniqueCount="199">
   <si>
     <t xml:space="preserve">Ocupantes podran contender en</t>
   </si>
@@ -553,7 +553,7 @@
     <t xml:space="preserve">2sep</t>
   </si>
   <si>
-    <t xml:space="preserve">12mayo2020 reforma const para adoptar reeleccion consecutiva</t>
+    <t xml:space="preserve">12mayo2020 reforma const para adoptar reeleccion consecutiva luego SCJN invalido la reforma 24nov2020</t>
   </si>
   <si>
     <t xml:space="preserve">Yucatán</t>
@@ -815,14 +815,14 @@
   <dimension ref="A1:BA101"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E82" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A82" activeCellId="0" sqref="A82"/>
+      <selection pane="bottomRight" activeCell="E95" activeCellId="0" sqref="E95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="3.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.47"/>
@@ -13626,8 +13626,8 @@
       <c r="D95" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E95" s="6" t="n">
-        <v>2025</v>
+      <c r="E95" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="F95" s="6" t="n">
         <v>2</v>
@@ -13735,7 +13735,7 @@
         <v>50</v>
       </c>
       <c r="AO95" s="6" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="AP95" s="6" t="n">
         <v>70</v>
@@ -14599,7 +14599,7 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -14633,7 +14633,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="44.28"/>

</xml_diff>